<commit_message>
pendulum experiment new added
</commit_message>
<xml_diff>
--- a/nf1.xlsx
+++ b/nf1.xlsx
@@ -432,28 +432,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.134100171</v>
+        <v>4.353290908</v>
       </c>
       <c r="C2">
-        <v>5.824931474</v>
+        <v>5.104107506</v>
       </c>
       <c r="D2">
-        <v>2.759151459</v>
+        <v>4.570819855</v>
       </c>
       <c r="E2">
-        <v>1.479027748</v>
+        <v>2.758747578</v>
       </c>
       <c r="F2">
-        <v>0.6908313029999995</v>
+        <v>0.7508165980000001</v>
       </c>
       <c r="G2">
-        <v>0.6235382451897624</v>
+        <v>0.5049157875049435</v>
       </c>
       <c r="H2">
-        <v>0.09923919392879692</v>
+        <v>0.0803598434265488</v>
       </c>
       <c r="I2">
-        <v>9.095107995098466</v>
+        <v>8.368468843012426</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -461,28 +461,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.824931474</v>
+        <v>7.054631072</v>
       </c>
       <c r="C3">
-        <v>6.514762969</v>
+        <v>7.804447965</v>
       </c>
       <c r="D3">
-        <v>1.479027748</v>
+        <v>0.2230691910000001</v>
       </c>
       <c r="E3">
-        <v>0.5918855667</v>
+        <v>0.1952342987</v>
       </c>
       <c r="F3">
-        <v>0.689831495</v>
+        <v>0.7498168929999993</v>
       </c>
       <c r="G3">
-        <v>0.9158269071540205</v>
+        <v>0.133281627780859</v>
       </c>
       <c r="H3">
-        <v>0.1457583792901246</v>
+        <v>0.02121242988465779</v>
       </c>
       <c r="I3">
-        <v>9.108289999399908</v>
+        <v>8.379626233867196</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -490,28 +490,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6.574748298999999</v>
+        <v>9.004154965</v>
       </c>
       <c r="C4">
-        <v>7.264579827</v>
+        <v>9.753971722999999</v>
       </c>
       <c r="D4">
-        <v>0.5705480575999999</v>
+        <v>0.04548645019999999</v>
       </c>
       <c r="E4">
-        <v>0.3810100554999999</v>
+        <v>0.0364074707</v>
       </c>
       <c r="F4">
-        <v>0.6898315280000009</v>
+        <v>0.7498167579999997</v>
       </c>
       <c r="G4">
-        <v>0.4037716362736964</v>
+        <v>0.2226404912090963</v>
       </c>
       <c r="H4">
-        <v>0.06426225179326163</v>
+        <v>0.03543433470833535</v>
       </c>
       <c r="I4">
-        <v>9.108289563679637</v>
+        <v>8.379627742568523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version of pendulum added
</commit_message>
<xml_diff>
--- a/nf1.xlsx
+++ b/nf1.xlsx
@@ -432,28 +432,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4.353290908</v>
+        <v>5.824931474</v>
       </c>
       <c r="C2">
-        <v>5.104107506</v>
+        <v>6.544755634</v>
       </c>
       <c r="D2">
-        <v>4.570819855</v>
+        <v>1.479027748</v>
       </c>
       <c r="E2">
-        <v>2.758747578</v>
+        <v>0.5702867508</v>
       </c>
       <c r="F2">
-        <v>0.7508165980000001</v>
+        <v>0.7198241599999999</v>
       </c>
       <c r="G2">
-        <v>0.5049157875049435</v>
+        <v>0.9530009179505683</v>
       </c>
       <c r="H2">
-        <v>0.0803598434265488</v>
+        <v>0.1516748068629467</v>
       </c>
       <c r="I2">
-        <v>8.368468843012426</v>
+        <v>8.728778021537353</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -461,28 +461,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>7.054631072</v>
+        <v>6.544755634</v>
       </c>
       <c r="C3">
-        <v>7.804447965</v>
+        <v>7.264579827</v>
       </c>
       <c r="D3">
-        <v>0.2230691910000001</v>
+        <v>0.5702867508</v>
       </c>
       <c r="E3">
-        <v>0.1952342987</v>
+        <v>0.3810100555</v>
       </c>
       <c r="F3">
-        <v>0.7498168929999993</v>
+        <v>0.719824193</v>
       </c>
       <c r="G3">
-        <v>0.133281627780859</v>
+        <v>0.4033135387425803</v>
       </c>
       <c r="H3">
-        <v>0.02121242988465779</v>
+        <v>0.06418934330676629</v>
       </c>
       <c r="I3">
-        <v>8.379626233867196</v>
+        <v>8.72877762137065</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -490,28 +490,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>9.004154965</v>
+        <v>7.804447965</v>
       </c>
       <c r="C4">
-        <v>9.753971722999999</v>
+        <v>8.524272157</v>
       </c>
       <c r="D4">
-        <v>0.04548645019999999</v>
+        <v>0.1952342987</v>
       </c>
       <c r="E4">
-        <v>0.0364074707</v>
+        <v>0.1958169937</v>
       </c>
       <c r="F4">
-        <v>0.7498167579999997</v>
+        <v>0.7198241920000008</v>
       </c>
       <c r="G4">
-        <v>0.2226404912090963</v>
+        <v>-0.002980148346680622</v>
       </c>
       <c r="H4">
-        <v>0.03543433470833535</v>
+        <v>-0.0004743053405213604</v>
       </c>
       <c r="I4">
-        <v>8.379627742568523</v>
+        <v>8.728777633496902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>